<commit_message>
Initial commit of Component Required Field Validation
</commit_message>
<xml_diff>
--- a/Validation/Component/Component Required Field Validation Report - Template.xlsx
+++ b/Validation/Component/Component Required Field Validation Report - Template.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cbuck\Documents\Projects\NNWW\AssetWorks Conversion\Validation\Component\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\REPOS\AssetWorksConversion\Validation\Component\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5952"/>
   </bookViews>
   <sheets>
-    <sheet name="Reqd Field Validation" sheetId="1" r:id="rId1"/>
+    <sheet name="RequiredFields" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>AssetID</t>
   </si>
@@ -41,21 +41,21 @@
     <t>Description</t>
   </si>
   <si>
+    <t>ModelYear</t>
+  </si>
+  <si>
+    <t>ManufacturerID</t>
+  </si>
+  <si>
+    <t>ModelID</t>
+  </si>
+  <si>
     <t>EquipmentType</t>
   </si>
   <si>
     <t>PMProgramType</t>
   </si>
   <si>
-    <t>ModelYear</t>
-  </si>
-  <si>
-    <t>ManufacturerID</t>
-  </si>
-  <si>
-    <t>ModelID</t>
-  </si>
-  <si>
     <t>MeterTypesClass</t>
   </si>
   <si>
@@ -74,7 +74,7 @@
     <t>Resources</t>
   </si>
   <si>
-    <t>AssetCategoryID</t>
+    <t>AssetcategoryID</t>
   </si>
   <si>
     <t>AssignedPM</t>
@@ -83,24 +83,35 @@
     <t>AssignedRepair</t>
   </si>
   <si>
+    <t>PreferredPMShift</t>
+  </si>
+  <si>
     <t>StationLocation</t>
   </si>
   <si>
-    <t>PreferredPMShift</t>
-  </si>
-  <si>
     <t>DepartmentID</t>
   </si>
   <si>
     <t>DepartmentForPM</t>
+  </si>
+  <si>
+    <t>WorkOrders</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -128,8 +139,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,86 +423,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W1"/>
+  <dimension ref="A1:X1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="8.88671875" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="W1" s="2" t="s">
         <v>22</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>